<commit_message>
VCA-4: update temp BOM spreadsheet
</commit_message>
<xml_diff>
--- a/modules/VCA-4/VCA-4-BOM.xlsx
+++ b/modules/VCA-4/VCA-4-BOM.xlsx
@@ -1,38 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\VCA-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\VCA-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2B96D3-76CF-4069-A75B-7C8E42710305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2EDA6381-A407-47C0-AB20-26E957419FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="780" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="VCA-4-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="231">
   <si>
     <t>Ref</t>
   </si>
@@ -229,7 +217,7 @@
     <t>H1 H5 H6 H10</t>
   </si>
   <si>
-    <t>HW_Screw_M3x0.50x6</t>
+    <t>Screw_M3x0.50x6</t>
   </si>
   <si>
     <t>Machine screw, M3x0.50x6</t>
@@ -238,7 +226,7 @@
     <t>H3 H8</t>
   </si>
   <si>
-    <t>HW_Standoff_F-F_11mm_M3x0.50</t>
+    <t>Standoff_F-F_11mm_M3x0.50</t>
   </si>
   <si>
     <t>Standoff, 11mm, female-female, M3x0.50</t>
@@ -310,12 +298,36 @@
     <t>Generic connector, single row, 01x24, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
+    <t>https://www.mouser.ca/datasheet/2/445/61303211821-1717799.pdf</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/598</t>
+  </si>
+  <si>
+    <t>710-61303211821</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/61303211821?qs=ZtY9WdtwX55M%2FH%2FSrHZ9xA%3D%3D</t>
+  </si>
+  <si>
     <t>J14 J16</t>
   </si>
   <si>
     <t>Conn_Header_24</t>
   </si>
   <si>
+    <t>https://www.amphenol-icc.com/media/wysiwyg/files/documentation/datasheet/boardwiretoboard/bwb_econostik_254headers.pdf</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/392</t>
+  </si>
+  <si>
+    <t>649-1012937893601BLF</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/649-1012937893601BLF</t>
+  </si>
+  <si>
     <t>J17</t>
   </si>
   <si>
@@ -337,6 +349,12 @@
     <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/61201021621?qs=%2Fha2pyFadugkhyfdWLPRIwz9kroMfF%252BXZWEETFcVSqiQRaqHzEC2RQ%3D%3D</t>
   </si>
   <si>
+    <t>523-G821EU210AAL10Y</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/523-G821EU210AAL10Y</t>
+  </si>
+  <si>
     <t>J18</t>
   </si>
   <si>
@@ -691,16 +709,16 @@
     <t>Have</t>
   </si>
   <si>
-    <t>Need</t>
-  </si>
-  <si>
-    <t>Ordered?</t>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1230,22 +1248,16 @@
   <dxfs count="1">
     <dxf>
       <font>
-        <color rgb="FFA80000"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF8F8F"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFA80000"/>
-      <color rgb="FFFF8F8F"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1553,20 +1565,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="4.1328125" customWidth="1"/>
+    <col min="2" max="5" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1574,13 +1586,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -1631,7 +1643,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1718,7 +1730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1760,7 +1772,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1802,7 +1814,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1841,7 +1853,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1849,7 +1861,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -1862,7 +1874,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1910,7 +1922,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -1921,7 +1933,7 @@
         <v>12</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E14" si="1">MAX(B9-C9-D9,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" t="s">
@@ -1967,7 +1979,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -1978,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" t="s">
@@ -1987,10 +1999,31 @@
       <c r="I10" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="J10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M10" t="s">
+        <v>87</v>
+      </c>
+      <c r="N10">
+        <v>598</v>
+      </c>
+      <c r="O10" t="s">
+        <v>93</v>
+      </c>
+      <c r="P10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>94</v>
+      </c>
+      <c r="R10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1999,41 +2032,59 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="I11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="J11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M11" t="s">
+        <v>87</v>
+      </c>
+      <c r="N11">
+        <v>392</v>
+      </c>
+      <c r="O11" t="s">
+        <v>99</v>
+      </c>
+      <c r="P11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>100</v>
+      </c>
+      <c r="R11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
       <c r="E12">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="I12" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="J12" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="K12" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="L12">
         <v>61201021621</v>
@@ -2042,15 +2093,24 @@
         <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="O12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+      <c r="P12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>109</v>
+      </c>
+      <c r="R12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2059,19 +2119,40 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="I13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+      <c r="J13" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13">
+        <v>598</v>
+      </c>
+      <c r="O13" t="s">
+        <v>93</v>
+      </c>
+      <c r="P13" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>94</v>
+      </c>
+      <c r="R13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2080,19 +2161,40 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="I14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+      <c r="J14" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" t="s">
+        <v>87</v>
+      </c>
+      <c r="N14">
+        <v>392</v>
+      </c>
+      <c r="O14" t="s">
+        <v>99</v>
+      </c>
+      <c r="P14" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>100</v>
+      </c>
+      <c r="R14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -2105,81 +2207,78 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="G15" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="H15" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="I15" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J15" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="K15" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="L15" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="M15" t="s">
         <v>36</v>
       </c>
       <c r="N15" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="O15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
-      <c r="D16">
-        <v>10</v>
-      </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="G16" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I16" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J16" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K16" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L16" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="M16" t="s">
         <v>36</v>
       </c>
       <c r="N16" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="O16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2192,36 +2291,36 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I17" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J17" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K17" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L17" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="M17" t="s">
         <v>36</v>
       </c>
       <c r="N17" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="O17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -2234,33 +2333,33 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="I18" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J18" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="K18" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="L18" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="M18" t="s">
         <v>36</v>
       </c>
       <c r="N18" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="O18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2273,36 +2372,36 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I19" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J19" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K19" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L19" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="M19" t="s">
         <v>36</v>
       </c>
       <c r="N19" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="O19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -2315,36 +2414,36 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I20" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J20" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K20" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L20" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="M20" t="s">
         <v>36</v>
       </c>
       <c r="N20" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="O20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -2357,78 +2456,75 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I21" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J21" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K21" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L21" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="M21" t="s">
         <v>36</v>
       </c>
       <c r="N21" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="O21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
-      <c r="D22">
-        <v>10</v>
-      </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="G22" s="1">
         <v>0.01</v>
       </c>
       <c r="I22" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J22" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="K22" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="L22" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M22" t="s">
         <v>36</v>
       </c>
       <c r="N22" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="O22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -2441,36 +2537,36 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="G23" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I23" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J23" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K23" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L23" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="M23" t="s">
         <v>36</v>
       </c>
       <c r="N23" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="O23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B24">
         <v>17</v>
@@ -2483,36 +2579,36 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I24" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J24" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K24" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L24" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="M24" t="s">
         <v>36</v>
       </c>
       <c r="N24" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="O24" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -2525,36 +2621,36 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="G25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="I25" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J25" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="K25" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="L25" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="M25" t="s">
         <v>36</v>
       </c>
       <c r="N25" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="O25" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -2567,54 +2663,54 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="G26" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="I26" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="J26" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="K26" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="L26" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="M26" t="s">
         <v>22</v>
       </c>
       <c r="N26" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="O26" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="P26" t="s">
         <v>36</v>
       </c>
       <c r="Q26" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="R26" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="S26" t="s">
         <v>24</v>
       </c>
       <c r="T26" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="U26" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -2627,45 +2723,45 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="G27" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="I27" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="J27" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="K27" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="L27" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="M27" t="s">
         <v>24</v>
       </c>
       <c r="N27" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="O27" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="P27" t="s">
         <v>22</v>
       </c>
       <c r="Q27" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="R27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2678,84 +2774,84 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="G28" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="I28" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="J28" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="K28" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="L28" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="M28" t="s">
         <v>36</v>
       </c>
       <c r="N28" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="O28" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="I29" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="J29" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="K29" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="L29" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="M29" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="N29" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="O29" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="P29" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="Q29" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="R29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="B30">
         <v>4</v>
@@ -2768,37 +2864,36 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="I30" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="J30" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="K30" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="L30" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="M30" t="s">
         <v>36</v>
       </c>
       <c r="N30" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="O30" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E30">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$E2&gt;0</formula>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>